<commit_message>
add outbreak info hits
</commit_message>
<xml_diff>
--- a/vcf-files/meta-data.xlsx
+++ b/vcf-files/meta-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikos\INABcloud\COVID-19\Lymata\sars-sewage\Thessaloniki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nikospech\INAB\lineages-in-bam\vcf-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FB694E-5B47-4A03-8211-646D587F9E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5534498-0FA1-41AC-A2C3-AB90321C487E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3090" yWindow="855" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -229,6 +229,21 @@
   </si>
   <si>
     <t>11-17 June 2021</t>
+  </si>
+  <si>
+    <t>L21_S1</t>
+  </si>
+  <si>
+    <t>L22N_S2</t>
+  </si>
+  <si>
+    <t>L22Q_S1</t>
+  </si>
+  <si>
+    <t>17-23  June 2021</t>
+  </si>
+  <si>
+    <t>24-30 June 2021</t>
   </si>
 </sst>
 </file>
@@ -578,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,6 +1145,30 @@
         <v>67</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>